<commit_message>
Changed the Readme.md file
</commit_message>
<xml_diff>
--- a/backend/uploads/excel/ASHLEY_GILL_parsed.xlsx
+++ b/backend/uploads/excel/ASHLEY_GILL_parsed.xlsx
@@ -463,7 +463,7 @@
         <v>skills</v>
       </c>
       <c r="B8" t="str">
-        <v>Communication, Presentation Skills, Customer Service, Rapport Building, Problem Solving, Relationship Management, Teamwork, Administration, Planning, Time Management, Data Collection, Travel Industry Knowledge, Initiative, Bookkeeping, Adaptability, Sales, Financial Acumen, Upselling</v>
+        <v>Business Studies, Business Planning, Sales Promotion, Marketing, Business Operations Management, Effective Communication, Presentation Skills, Customer Service, Teamwork, Administration, Time Management, Data Gathering, Travel Consultancy, International Travel Experience, Initiative, Bookkeeping, Sales Knowledge, Up-selling, Financial Processes</v>
       </c>
     </row>
     <row r="9">
@@ -471,7 +471,7 @@
         <v>languages</v>
       </c>
       <c r="B9" t="str">
-        <v>Spanish (Fluent), French (Semi-fluent), English (Native)</v>
+        <v>Spanish (Fluent), French (Semi-fluent), English (Professional Working Proficiency)</v>
       </c>
     </row>
     <row r="10">

</xml_diff>